<commit_message>
dictionary based introduction + CBoss explanation, still missing CST explanation
</commit_message>
<xml_diff>
--- a/Datasets_metadata_charts.xlsx
+++ b/Datasets_metadata_charts.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ismail\Desktop\OVGU\DKE Subjects\Master-Thesis\"/>
@@ -18,15 +18,15 @@
     <sheet name="type" sheetId="8" r:id="rId4"/>
     <sheet name="Datasets_metadata" sheetId="1" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="125">
   <si>
     <t>dataset</t>
   </si>
@@ -389,6 +389,18 @@
   </si>
   <si>
     <t>(All)</t>
+  </si>
+  <si>
+    <t>6-10</t>
+  </si>
+  <si>
+    <t>11-15</t>
+  </si>
+  <si>
+    <t>16-30</t>
+  </si>
+  <si>
+    <t>31-50</t>
   </si>
 </sst>
 </file>
@@ -900,7 +912,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -913,6 +925,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -992,11 +1006,15 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="2400" b="0"/>
+              <a:defRPr/>
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="2400" b="0"/>
-              <a:t>Train Set Size</a:t>
+              <a:t>Train Set </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400" b="0" i="0" baseline="0"/>
+              <a:t>Size</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1021,6 +1039,13 @@
             <a:solidFill>
               <a:schemeClr val="tx1"/>
             </a:solidFill>
+            <a:effectLst>
+              <a:glow>
+                <a:schemeClr val="accent1">
+                  <a:alpha val="40000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
@@ -1031,7 +1056,18 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:dLblPos val="outEnd"/>
+            <c:txPr>
+              <a:bodyPr wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -1101,7 +1137,6 @@
           </c:val>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
           <c:showCatName val="0"/>
@@ -1109,22 +1144,32 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="1819836608"/>
-        <c:axId val="1819851296"/>
+        <c:gapWidth val="75"/>
+        <c:axId val="-1855303552"/>
+        <c:axId val="-1855300288"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1819836608"/>
+        <c:axId val="-1855303552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1819851296"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1855300288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1132,7 +1177,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1819851296"/>
+        <c:axId val="-1855300288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -1141,10 +1186,20 @@
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1819836608"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1855303552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1195,7 +1250,7 @@
               <a:defRPr sz="2400" b="0"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="2400" b="0"/>
               <a:t>Series Length</a:t>
             </a:r>
           </a:p>
@@ -1218,6 +1273,13 @@
             <a:solidFill>
               <a:schemeClr val="tx1"/>
             </a:solidFill>
+            <a:effectLst>
+              <a:glow>
+                <a:schemeClr val="accent1">
+                  <a:alpha val="40000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
@@ -1228,7 +1290,18 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:dLblPos val="outEnd"/>
+            <c:txPr>
+              <a:bodyPr wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -1298,7 +1371,6 @@
           </c:val>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
           <c:showCatName val="0"/>
@@ -1306,22 +1378,32 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="1836902592"/>
-        <c:axId val="1836915648"/>
+        <c:gapWidth val="75"/>
+        <c:axId val="-1693831072"/>
+        <c:axId val="-1693837600"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1836902592"/>
+        <c:axId val="-1693831072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1836915648"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1693837600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1329,7 +1411,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1836915648"/>
+        <c:axId val="-1693837600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -1338,10 +1420,20 @@
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1836902592"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1693831072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1392,7 +1484,7 @@
               <a:defRPr sz="2400" b="0"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="2400" b="0"/>
               <a:t>Number of Classes</a:t>
             </a:r>
           </a:p>
@@ -1415,6 +1507,13 @@
             <a:solidFill>
               <a:schemeClr val="tx1"/>
             </a:solidFill>
+            <a:effectLst>
+              <a:glow>
+                <a:schemeClr val="accent1">
+                  <a:alpha val="40000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
@@ -1425,7 +1524,18 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:dLblPos val="outEnd"/>
+            <c:txPr>
+              <a:bodyPr wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -1458,16 +1568,16 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>6-10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15</c:v>
+                  <c:v>11-15</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30</c:v>
+                  <c:v>16-30</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>50</c:v>
+                  <c:v>31-50</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>50+</c:v>
@@ -1513,7 +1623,6 @@
           </c:val>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
           <c:showCatName val="0"/>
@@ -1521,22 +1630,32 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="1836902048"/>
-        <c:axId val="1836906400"/>
+        <c:gapWidth val="75"/>
+        <c:axId val="-1796123632"/>
+        <c:axId val="-1796119824"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1836902048"/>
+        <c:axId val="-1796123632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1836906400"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1796119824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1544,19 +1663,29 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1836906400"/>
+        <c:axId val="-1796119824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="35"/>
+          <c:max val="25"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1836902048"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1796123632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1611,7 +1740,7 @@
               <a:defRPr sz="2400" b="0"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="2400" b="0"/>
               <a:t>Problem Type</a:t>
             </a:r>
           </a:p>
@@ -1628,6 +1757,13 @@
           <a:solidFill>
             <a:schemeClr val="tx1"/>
           </a:solidFill>
+          <a:effectLst>
+            <a:glow>
+              <a:schemeClr val="accent1">
+                <a:alpha val="40000"/>
+              </a:schemeClr>
+            </a:glow>
+          </a:effectLst>
         </c:spPr>
         <c:marker>
           <c:symbol val="none"/>
@@ -1649,12 +1785,11 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr/>
+                <a:defRPr sz="1600"/>
               </a:pPr>
               <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
-          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
           <c:showCatName val="0"/>
@@ -1693,6 +1828,13 @@
             <a:solidFill>
               <a:schemeClr val="tx1"/>
             </a:solidFill>
+            <a:effectLst>
+              <a:glow>
+                <a:schemeClr val="accent1">
+                  <a:alpha val="40000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
@@ -1710,12 +1852,11 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1600"/>
                 </a:pPr>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -1833,7 +1974,6 @@
           </c:val>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
           <c:showCatName val="0"/>
@@ -1841,22 +1981,32 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="1838030624"/>
-        <c:axId val="1838038784"/>
+        <c:gapWidth val="75"/>
+        <c:axId val="-2062988688"/>
+        <c:axId val="-2062988144"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1838030624"/>
+        <c:axId val="-2062988688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1838038784"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2062988144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1864,19 +2014,29 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1838038784"/>
+        <c:axId val="-2062988144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="20"/>
+          <c:max val="25"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1838030624"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2062988688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3115,7 +3275,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9">
   <location ref="A3:B18" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="11">
     <pivotField dataField="1" showAll="0"/>
@@ -3236,6 +3396,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K78" totalsRowShown="0">
   <autoFilter ref="A1:K78"/>
+  <sortState ref="A2:K78">
+    <sortCondition ref="J1:J78"/>
+  </sortState>
   <tableColumns count="11">
     <tableColumn id="1" name="dataset"/>
     <tableColumn id="2" name="uea_ucr"/>
@@ -4275,7 +4438,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A7"/>
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4356,7 +4519,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4431,7 +4594,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4445,7 +4608,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+      <c r="A2" s="8">
         <v>2</v>
       </c>
       <c r="B2" s="3">
@@ -4453,7 +4616,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+      <c r="A3" s="8">
         <v>3</v>
       </c>
       <c r="B3" s="3">
@@ -4461,7 +4624,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
+      <c r="A4" s="8">
         <v>4</v>
       </c>
       <c r="B4" s="3">
@@ -4469,7 +4632,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+      <c r="A5" s="8">
         <v>5</v>
       </c>
       <c r="B5" s="3">
@@ -4477,39 +4640,39 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
-        <v>10</v>
+      <c r="A6" s="8" t="s">
+        <v>121</v>
       </c>
       <c r="B6" s="3">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
-        <v>15</v>
+      <c r="A7" s="8" t="s">
+        <v>122</v>
       </c>
       <c r="B7" s="3">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
-        <v>30</v>
+      <c r="A8" s="8" t="s">
+        <v>123</v>
       </c>
       <c r="B8" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
-        <v>50</v>
+      <c r="A9" s="8" t="s">
+        <v>124</v>
       </c>
       <c r="B9" s="3">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="9" t="s">
         <v>116</v>
       </c>
       <c r="B10" s="4">
@@ -4536,7 +4699,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4692,12 +4855,12 @@
   <dimension ref="A1:O78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+      <selection activeCell="A4" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="1" max="1" width="25.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.44140625" customWidth="1"/>
     <col min="3" max="3" width="9.109375" customWidth="1"/>
     <col min="4" max="4" width="10.6640625" customWidth="1"/>
@@ -4754,28 +4917,28 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>79</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>79</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
       </c>
       <c r="D2">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="E2">
-        <v>100</v>
+        <v>208</v>
       </c>
       <c r="F2">
-        <v>1460</v>
+        <v>2000</v>
       </c>
       <c r="G2">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="H2" t="s">
-        <v>12</v>
+        <v>80</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -4798,34 +4961,34 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>81</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>81</v>
       </c>
       <c r="C3" t="b">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>15</v>
+        <v>104</v>
       </c>
       <c r="E3">
-        <v>15</v>
+        <v>208</v>
       </c>
       <c r="F3">
-        <v>640</v>
+        <v>2000</v>
       </c>
       <c r="G3">
-        <v>3</v>
+        <v>52</v>
       </c>
       <c r="H3" t="s">
-        <v>15</v>
+        <v>80</v>
       </c>
       <c r="I3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K3" t="b">
         <v>1</v>
@@ -4842,34 +5005,34 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>82</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>82</v>
       </c>
       <c r="C4" t="b">
         <v>1</v>
       </c>
       <c r="D4">
-        <v>40</v>
+        <v>104</v>
       </c>
       <c r="E4">
-        <v>40</v>
+        <v>208</v>
       </c>
       <c r="F4">
-        <v>100</v>
+        <v>2000</v>
       </c>
       <c r="G4">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="H4" t="s">
-        <v>18</v>
+        <v>80</v>
       </c>
       <c r="I4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="K4" t="b">
         <v>1</v>
@@ -4886,28 +5049,28 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="C5" t="b">
         <v>1</v>
       </c>
       <c r="D5">
-        <v>30</v>
+        <v>1800</v>
       </c>
       <c r="E5">
-        <v>30</v>
+        <v>1965</v>
       </c>
       <c r="F5">
-        <v>470</v>
+        <v>750</v>
       </c>
       <c r="G5">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="H5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I5" t="s">
         <v>13</v>
@@ -4930,28 +5093,28 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>73</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>73</v>
       </c>
       <c r="C6" t="b">
         <v>1</v>
       </c>
       <c r="D6">
-        <v>60</v>
+        <v>1800</v>
       </c>
       <c r="E6">
-        <v>60</v>
+        <v>1965</v>
       </c>
       <c r="F6">
-        <v>577</v>
+        <v>750</v>
       </c>
       <c r="G6">
-        <v>4</v>
+        <v>42</v>
       </c>
       <c r="H6" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="I6" t="s">
         <v>13</v>
@@ -4974,28 +5137,28 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>77</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>77</v>
       </c>
       <c r="C7" t="b">
         <v>1</v>
       </c>
       <c r="D7">
-        <v>20</v>
+        <v>214</v>
       </c>
       <c r="E7">
-        <v>345</v>
+        <v>1896</v>
       </c>
       <c r="F7">
-        <v>24</v>
+        <v>1024</v>
       </c>
       <c r="G7">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="H7" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
       <c r="I7" t="s">
         <v>13</v>
@@ -5004,7 +5167,7 @@
         <v>1</v>
       </c>
       <c r="K7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O7">
         <v>15</v>
@@ -5012,28 +5175,28 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="C8" t="b">
         <v>1</v>
       </c>
       <c r="D8">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="E8">
-        <v>1380</v>
+        <v>186</v>
       </c>
       <c r="F8">
-        <v>1639</v>
+        <v>201</v>
       </c>
       <c r="G8">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="H8" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="I8" t="s">
         <v>13</v>
@@ -5042,7 +5205,7 @@
         <v>1</v>
       </c>
       <c r="K8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O8">
         <v>30</v>
@@ -5050,28 +5213,28 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="C9" t="b">
         <v>1</v>
       </c>
       <c r="D9">
-        <v>28</v>
+        <v>362</v>
       </c>
       <c r="E9">
-        <v>28</v>
+        <v>362</v>
       </c>
       <c r="F9">
-        <v>286</v>
+        <v>1250</v>
       </c>
       <c r="G9">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="H9" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="I9" t="s">
         <v>13</v>
@@ -5088,28 +5251,28 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="C10" t="b">
         <v>1</v>
       </c>
       <c r="D10">
-        <v>250</v>
+        <v>362</v>
       </c>
       <c r="E10">
-        <v>250</v>
+        <v>362</v>
       </c>
       <c r="F10">
-        <v>720</v>
+        <v>1250</v>
       </c>
       <c r="G10">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="H10" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="I10" t="s">
         <v>13</v>
@@ -5123,34 +5286,34 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="C11" t="b">
         <v>1</v>
       </c>
       <c r="D11">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="E11">
-        <v>72</v>
+        <v>100</v>
       </c>
       <c r="F11">
-        <v>1197</v>
+        <v>1460</v>
       </c>
       <c r="G11">
+        <v>10</v>
+      </c>
+      <c r="H11" t="s">
         <v>12</v>
       </c>
-      <c r="H11" t="s">
-        <v>18</v>
-      </c>
       <c r="I11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J11">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="K11" t="b">
         <v>1</v>
@@ -5158,34 +5321,34 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="C12" t="b">
         <v>1</v>
       </c>
       <c r="D12">
-        <v>60</v>
+        <v>25000</v>
       </c>
       <c r="E12">
-        <v>40</v>
+        <v>25000</v>
       </c>
       <c r="F12">
-        <v>270</v>
+        <v>600</v>
       </c>
       <c r="G12">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H12" t="s">
         <v>30</v>
       </c>
       <c r="I12" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J12">
-        <v>1345</v>
+        <v>1</v>
       </c>
       <c r="K12" t="b">
         <v>1</v>
@@ -5193,25 +5356,25 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
       <c r="C13" t="b">
         <v>1</v>
       </c>
       <c r="D13">
-        <v>322</v>
+        <v>70</v>
       </c>
       <c r="E13">
-        <v>139</v>
+        <v>73</v>
       </c>
       <c r="F13">
-        <v>512</v>
+        <v>319</v>
       </c>
       <c r="G13">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H13" t="s">
         <v>22</v>
@@ -5228,28 +5391,28 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>83</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>83</v>
       </c>
       <c r="C14" t="b">
         <v>1</v>
       </c>
       <c r="D14">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="E14">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="F14">
-        <v>96</v>
+        <v>144</v>
       </c>
       <c r="G14">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H14" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="I14" t="s">
         <v>13</v>
@@ -5263,28 +5426,28 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C15" t="b">
         <v>1</v>
       </c>
       <c r="D15">
-        <v>500</v>
+        <v>8926</v>
       </c>
       <c r="E15">
-        <v>4500</v>
+        <v>7711</v>
       </c>
       <c r="F15">
-        <v>140</v>
+        <v>96</v>
       </c>
       <c r="G15">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H15" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I15" t="s">
         <v>13</v>
@@ -5298,28 +5461,28 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>92</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>92</v>
       </c>
       <c r="C16" t="b">
         <v>1</v>
       </c>
       <c r="D16">
-        <v>23</v>
+        <v>450</v>
       </c>
       <c r="E16">
-        <v>861</v>
+        <v>450</v>
       </c>
       <c r="F16">
-        <v>136</v>
+        <v>1500</v>
       </c>
       <c r="G16">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H16" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I16" t="s">
         <v>13</v>
@@ -5333,28 +5496,28 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="C17" t="b">
         <v>1</v>
       </c>
       <c r="D17">
-        <v>8926</v>
+        <v>30</v>
       </c>
       <c r="E17">
-        <v>7711</v>
+        <v>30</v>
       </c>
       <c r="F17">
-        <v>96</v>
+        <v>470</v>
       </c>
       <c r="G17">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H17" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="I17" t="s">
         <v>13</v>
@@ -5363,33 +5526,33 @@
         <v>1</v>
       </c>
       <c r="K17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="C18" t="b">
         <v>1</v>
       </c>
       <c r="D18">
-        <v>362</v>
+        <v>450</v>
       </c>
       <c r="E18">
-        <v>362</v>
+        <v>450</v>
       </c>
       <c r="F18">
-        <v>1250</v>
+        <v>1500</v>
       </c>
       <c r="G18">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H18" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="I18" t="s">
         <v>13</v>
@@ -5403,28 +5566,28 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C19" t="b">
         <v>1</v>
       </c>
       <c r="D19">
-        <v>362</v>
+        <v>500</v>
       </c>
       <c r="E19">
-        <v>362</v>
+        <v>4500</v>
       </c>
       <c r="F19">
-        <v>1250</v>
+        <v>140</v>
       </c>
       <c r="G19">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H19" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="I19" t="s">
         <v>13</v>
@@ -5433,39 +5596,39 @@
         <v>1</v>
       </c>
       <c r="K19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>87</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>87</v>
       </c>
       <c r="C20" t="b">
         <v>1</v>
       </c>
       <c r="D20">
-        <v>137</v>
+        <v>20</v>
       </c>
       <c r="E20">
-        <v>138</v>
+        <v>50</v>
       </c>
       <c r="F20">
-        <v>207</v>
+        <v>2844</v>
       </c>
       <c r="G20">
         <v>4</v>
       </c>
       <c r="H20" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I20" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J20">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K20" t="b">
         <v>1</v>
@@ -5473,10 +5636,10 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>74</v>
       </c>
       <c r="C21" t="b">
         <v>1</v>
@@ -5485,86 +5648,86 @@
         <v>30</v>
       </c>
       <c r="E21">
-        <v>270</v>
+        <v>30</v>
       </c>
       <c r="F21">
-        <v>65</v>
+        <v>570</v>
       </c>
       <c r="G21">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H21" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I21" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J21">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="C22" t="b">
         <v>1</v>
       </c>
       <c r="D22">
-        <v>261</v>
+        <v>40</v>
       </c>
       <c r="E22">
-        <v>263</v>
+        <v>1380</v>
       </c>
       <c r="F22">
-        <v>1751</v>
+        <v>1639</v>
       </c>
       <c r="G22">
         <v>4</v>
       </c>
       <c r="H22" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="I22" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J22">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="C23" t="b">
         <v>1</v>
       </c>
       <c r="D23">
-        <v>504</v>
+        <v>60</v>
       </c>
       <c r="E23">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="F23">
-        <v>1751</v>
+        <v>577</v>
       </c>
       <c r="G23">
         <v>4</v>
       </c>
       <c r="H23" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I23" t="s">
         <v>13</v>
@@ -5578,34 +5741,34 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>100</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>100</v>
       </c>
       <c r="C24" t="b">
         <v>1</v>
       </c>
       <c r="D24">
-        <v>5890</v>
+        <v>100</v>
       </c>
       <c r="E24">
-        <v>3524</v>
+        <v>100</v>
       </c>
       <c r="F24">
-        <v>62</v>
+        <v>275</v>
       </c>
       <c r="G24">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H24" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="I24" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J24">
-        <v>144</v>
+        <v>1</v>
       </c>
       <c r="K24" t="b">
         <v>1</v>
@@ -5613,34 +5776,34 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B25" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C25" t="b">
         <v>1</v>
       </c>
       <c r="D25">
-        <v>316</v>
+        <v>504</v>
       </c>
       <c r="E25">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="F25">
-        <v>50</v>
+        <v>1751</v>
       </c>
       <c r="G25">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H25" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="I25" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J25">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="K25" t="b">
         <v>1</v>
@@ -5648,28 +5811,28 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="B26" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="C26" t="b">
         <v>1</v>
       </c>
       <c r="D26">
-        <v>3601</v>
+        <v>17</v>
       </c>
       <c r="E26">
-        <v>1320</v>
+        <v>249</v>
       </c>
       <c r="F26">
-        <v>500</v>
+        <v>601</v>
       </c>
       <c r="G26">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H26" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="I26" t="s">
         <v>13</v>
@@ -5678,33 +5841,33 @@
         <v>1</v>
       </c>
       <c r="K26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="B27" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="C27" t="b">
         <v>1</v>
       </c>
       <c r="D27">
-        <v>3636</v>
+        <v>60</v>
       </c>
       <c r="E27">
-        <v>810</v>
+        <v>60</v>
       </c>
       <c r="F27">
-        <v>500</v>
+        <v>448</v>
       </c>
       <c r="G27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I27" t="s">
         <v>13</v>
@@ -5718,28 +5881,28 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="B28" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="C28" t="b">
         <v>1</v>
       </c>
       <c r="D28">
-        <v>150</v>
+        <v>62</v>
       </c>
       <c r="E28">
-        <v>2850</v>
+        <v>249</v>
       </c>
       <c r="F28">
-        <v>301</v>
+        <v>601</v>
       </c>
       <c r="G28">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H28" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="I28" t="s">
         <v>13</v>
@@ -5748,33 +5911,33 @@
         <v>1</v>
       </c>
       <c r="K28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="B29" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="C29" t="b">
         <v>1</v>
       </c>
       <c r="D29">
-        <v>28</v>
+        <v>375</v>
       </c>
       <c r="E29">
-        <v>2850</v>
+        <v>375</v>
       </c>
       <c r="F29">
-        <v>301</v>
+        <v>720</v>
       </c>
       <c r="G29">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H29" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="I29" t="s">
         <v>13</v>
@@ -5788,28 +5951,28 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>52</v>
+        <v>86</v>
       </c>
       <c r="B30" t="s">
-        <v>52</v>
+        <v>86</v>
       </c>
       <c r="C30" t="b">
         <v>1</v>
       </c>
       <c r="D30">
-        <v>18</v>
+        <v>375</v>
       </c>
       <c r="E30">
-        <v>186</v>
+        <v>375</v>
       </c>
       <c r="F30">
-        <v>201</v>
+        <v>720</v>
       </c>
       <c r="G30">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="H30" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="I30" t="s">
         <v>13</v>
@@ -5823,28 +5986,28 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>53</v>
+        <v>88</v>
       </c>
       <c r="B31" t="s">
-        <v>53</v>
+        <v>88</v>
       </c>
       <c r="C31" t="b">
         <v>1</v>
       </c>
       <c r="D31">
-        <v>109</v>
+        <v>375</v>
       </c>
       <c r="E31">
-        <v>105</v>
+        <v>375</v>
       </c>
       <c r="F31">
-        <v>431</v>
+        <v>720</v>
       </c>
       <c r="G31">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H31" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="I31" t="s">
         <v>13</v>
@@ -5858,34 +6021,34 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>54</v>
+        <v>94</v>
       </c>
       <c r="B32" t="s">
-        <v>54</v>
+        <v>94</v>
       </c>
       <c r="C32" t="b">
         <v>1</v>
       </c>
       <c r="D32">
-        <v>160</v>
+        <v>375</v>
       </c>
       <c r="E32">
-        <v>74</v>
+        <v>375</v>
       </c>
       <c r="F32">
-        <v>400</v>
+        <v>720</v>
       </c>
       <c r="G32">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H32" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="I32" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J32">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="K32" t="b">
         <v>1</v>
@@ -5893,34 +6056,34 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>55</v>
+        <v>98</v>
       </c>
       <c r="B33" t="s">
-        <v>55</v>
+        <v>98</v>
       </c>
       <c r="C33" t="b">
         <v>1</v>
       </c>
       <c r="D33">
-        <v>150</v>
+        <v>1000</v>
       </c>
       <c r="E33">
-        <v>850</v>
+        <v>8236</v>
       </c>
       <c r="F33">
-        <v>152</v>
+        <v>1024</v>
       </c>
       <c r="G33">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="H33" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="I33" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J33">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K33" t="b">
         <v>0</v>
@@ -5928,63 +6091,63 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="B34" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="C34" t="b">
         <v>1</v>
       </c>
       <c r="D34">
-        <v>204</v>
+        <v>20</v>
       </c>
       <c r="E34">
-        <v>205</v>
+        <v>345</v>
       </c>
       <c r="F34">
-        <v>405</v>
+        <v>24</v>
       </c>
       <c r="G34">
         <v>2</v>
       </c>
       <c r="H34" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="I34" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J34">
-        <v>61</v>
+        <v>1</v>
       </c>
       <c r="K34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="B35" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="C35" t="b">
         <v>1</v>
       </c>
       <c r="D35">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="E35">
-        <v>101</v>
+        <v>1252</v>
       </c>
       <c r="F35">
-        <v>3000</v>
+        <v>84</v>
       </c>
       <c r="G35">
         <v>2</v>
       </c>
       <c r="H35" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="I35" t="s">
         <v>13</v>
@@ -5998,28 +6161,28 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>58</v>
+        <v>95</v>
       </c>
       <c r="B36" t="s">
-        <v>58</v>
+        <v>95</v>
       </c>
       <c r="C36" t="b">
         <v>1</v>
       </c>
       <c r="D36">
-        <v>62</v>
+        <v>20</v>
       </c>
       <c r="E36">
-        <v>249</v>
+        <v>601</v>
       </c>
       <c r="F36">
-        <v>601</v>
+        <v>70</v>
       </c>
       <c r="G36">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H36" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
       <c r="I36" t="s">
         <v>13</v>
@@ -6033,28 +6196,28 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="B37" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="C37" t="b">
         <v>1</v>
       </c>
       <c r="D37">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E37">
-        <v>249</v>
+        <v>861</v>
       </c>
       <c r="F37">
-        <v>601</v>
+        <v>136</v>
       </c>
       <c r="G37">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H37" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
       <c r="I37" t="s">
         <v>13</v>
@@ -6063,33 +6226,33 @@
         <v>1</v>
       </c>
       <c r="K37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>61</v>
+        <v>101</v>
       </c>
       <c r="B38" t="s">
-        <v>61</v>
+        <v>101</v>
       </c>
       <c r="C38" t="b">
         <v>1</v>
       </c>
       <c r="D38">
-        <v>25000</v>
+        <v>23</v>
       </c>
       <c r="E38">
-        <v>25000</v>
+        <v>1139</v>
       </c>
       <c r="F38">
-        <v>600</v>
+        <v>82</v>
       </c>
       <c r="G38">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="H38" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="I38" t="s">
         <v>13</v>
@@ -6103,22 +6266,22 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>62</v>
+        <v>96</v>
       </c>
       <c r="B39" t="s">
-        <v>62</v>
+        <v>96</v>
       </c>
       <c r="C39" t="b">
         <v>1</v>
       </c>
       <c r="D39">
-        <v>67</v>
+        <v>27</v>
       </c>
       <c r="E39">
-        <v>1029</v>
+        <v>953</v>
       </c>
       <c r="F39">
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="G39">
         <v>2</v>
@@ -6138,28 +6301,28 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="B40" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="C40" t="b">
         <v>1</v>
       </c>
       <c r="D40">
-        <v>375</v>
+        <v>28</v>
       </c>
       <c r="E40">
-        <v>375</v>
+        <v>28</v>
       </c>
       <c r="F40">
-        <v>720</v>
+        <v>286</v>
       </c>
       <c r="G40">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H40" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="I40" t="s">
         <v>13</v>
@@ -6173,34 +6336,34 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="B41" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="C41" t="b">
         <v>1</v>
       </c>
       <c r="D41">
-        <v>180</v>
+        <v>28</v>
       </c>
       <c r="E41">
-        <v>180</v>
+        <v>2850</v>
       </c>
       <c r="F41">
-        <v>45</v>
+        <v>301</v>
       </c>
       <c r="G41">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="H41" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="I41" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K41" t="b">
         <v>1</v>
@@ -6208,28 +6371,28 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B42" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C42" t="b">
         <v>1</v>
       </c>
       <c r="D42">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="E42">
-        <v>61</v>
+        <v>101</v>
       </c>
       <c r="F42">
-        <v>637</v>
+        <v>3000</v>
       </c>
       <c r="G42">
         <v>2</v>
       </c>
       <c r="H42" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="I42" t="s">
         <v>13</v>
@@ -6238,33 +6401,33 @@
         <v>1</v>
       </c>
       <c r="K42" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>66</v>
+        <v>104</v>
       </c>
       <c r="B43" t="s">
-        <v>66</v>
+        <v>104</v>
       </c>
       <c r="C43" t="b">
         <v>1</v>
       </c>
       <c r="D43">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="E43">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="F43">
-        <v>319</v>
+        <v>234</v>
       </c>
       <c r="G43">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H43" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I43" t="s">
         <v>13</v>
@@ -6273,39 +6436,39 @@
         <v>1</v>
       </c>
       <c r="K43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B44" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C44" t="b">
         <v>1</v>
       </c>
       <c r="D44">
-        <v>2459</v>
+        <v>60</v>
       </c>
       <c r="E44">
-        <v>2466</v>
+        <v>61</v>
       </c>
       <c r="F44">
-        <v>36</v>
+        <v>637</v>
       </c>
       <c r="G44">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="H44" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="I44" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J44">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="K44" t="b">
         <v>0</v>
@@ -6313,28 +6476,28 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B45" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C45" t="b">
         <v>1</v>
       </c>
       <c r="D45">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="E45">
-        <v>60</v>
+        <v>1029</v>
       </c>
       <c r="F45">
-        <v>448</v>
+        <v>24</v>
       </c>
       <c r="G45">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H45" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I45" t="s">
         <v>13</v>
@@ -6348,28 +6511,28 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>69</v>
+        <v>32</v>
       </c>
       <c r="B46" t="s">
-        <v>69</v>
+        <v>32</v>
       </c>
       <c r="C46" t="b">
         <v>1</v>
       </c>
       <c r="D46">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="E46">
-        <v>1252</v>
+        <v>100</v>
       </c>
       <c r="F46">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="G46">
         <v>2</v>
       </c>
       <c r="H46" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="I46" t="s">
         <v>13</v>
@@ -6378,39 +6541,39 @@
         <v>1</v>
       </c>
       <c r="K46" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="B47" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="C47" t="b">
         <v>1</v>
       </c>
       <c r="D47">
-        <v>278</v>
+        <v>109</v>
       </c>
       <c r="E47">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="F47">
-        <v>3000</v>
+        <v>431</v>
       </c>
       <c r="G47">
         <v>2</v>
       </c>
       <c r="H47" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="I47" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J47">
-        <v>64</v>
+        <v>1</v>
       </c>
       <c r="K47" t="b">
         <v>1</v>
@@ -6418,34 +6581,34 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="B48" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="C48" t="b">
         <v>1</v>
       </c>
       <c r="D48">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="E48">
-        <v>180</v>
+        <v>2850</v>
       </c>
       <c r="F48">
-        <v>51</v>
+        <v>301</v>
       </c>
       <c r="G48">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H48" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="I48" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J48">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="K48" t="b">
         <v>1</v>
@@ -6453,28 +6616,28 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="B49" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="C49" t="b">
         <v>1</v>
       </c>
       <c r="D49">
-        <v>1800</v>
+        <v>180</v>
       </c>
       <c r="E49">
-        <v>1965</v>
+        <v>180</v>
       </c>
       <c r="F49">
-        <v>750</v>
+        <v>144</v>
       </c>
       <c r="G49">
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="H49" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I49" t="s">
         <v>13</v>
@@ -6488,28 +6651,28 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>73</v>
+        <v>27</v>
       </c>
       <c r="B50" t="s">
-        <v>73</v>
+        <v>27</v>
       </c>
       <c r="C50" t="b">
         <v>1</v>
       </c>
       <c r="D50">
-        <v>1800</v>
+        <v>250</v>
       </c>
       <c r="E50">
-        <v>1965</v>
+        <v>250</v>
       </c>
       <c r="F50">
-        <v>750</v>
+        <v>720</v>
       </c>
       <c r="G50">
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="H50" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I50" t="s">
         <v>13</v>
@@ -6523,25 +6686,25 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="B51" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="C51" t="b">
         <v>1</v>
       </c>
       <c r="D51">
-        <v>30</v>
+        <v>300</v>
       </c>
       <c r="E51">
-        <v>30</v>
+        <v>600</v>
       </c>
       <c r="F51">
-        <v>570</v>
+        <v>1500</v>
       </c>
       <c r="G51">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H51" t="s">
         <v>20</v>
@@ -6553,68 +6716,68 @@
         <v>1</v>
       </c>
       <c r="K51" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>75</v>
+        <v>31</v>
       </c>
       <c r="B52" t="s">
-        <v>75</v>
+        <v>31</v>
       </c>
       <c r="C52" t="b">
         <v>1</v>
       </c>
       <c r="D52">
-        <v>267</v>
+        <v>322</v>
       </c>
       <c r="E52">
-        <v>173</v>
+        <v>139</v>
       </c>
       <c r="F52">
-        <v>144</v>
+        <v>512</v>
       </c>
       <c r="G52">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H52" t="s">
-        <v>76</v>
+        <v>22</v>
       </c>
       <c r="I52" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J52">
-        <v>963</v>
+        <v>1</v>
       </c>
       <c r="K52" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="B53" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="C53" t="b">
         <v>1</v>
       </c>
       <c r="D53">
-        <v>214</v>
+        <v>613</v>
       </c>
       <c r="E53">
-        <v>1896</v>
+        <v>370</v>
       </c>
       <c r="F53">
-        <v>1024</v>
+        <v>235</v>
       </c>
       <c r="G53">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="H53" t="s">
-        <v>78</v>
+        <v>20</v>
       </c>
       <c r="I53" t="s">
         <v>13</v>
@@ -6623,33 +6786,33 @@
         <v>1</v>
       </c>
       <c r="K53" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>79</v>
+        <v>103</v>
       </c>
       <c r="B54" t="s">
-        <v>79</v>
+        <v>103</v>
       </c>
       <c r="C54" t="b">
         <v>1</v>
       </c>
       <c r="D54">
-        <v>104</v>
+        <v>1000</v>
       </c>
       <c r="E54">
-        <v>208</v>
+        <v>6164</v>
       </c>
       <c r="F54">
-        <v>2000</v>
+        <v>152</v>
       </c>
       <c r="G54">
-        <v>52</v>
+        <v>2</v>
       </c>
       <c r="H54" t="s">
-        <v>80</v>
+        <v>22</v>
       </c>
       <c r="I54" t="s">
         <v>13</v>
@@ -6658,33 +6821,33 @@
         <v>1</v>
       </c>
       <c r="K54" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
       <c r="B55" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
       <c r="C55" t="b">
         <v>1</v>
       </c>
       <c r="D55">
-        <v>104</v>
+        <v>3601</v>
       </c>
       <c r="E55">
-        <v>208</v>
+        <v>1320</v>
       </c>
       <c r="F55">
-        <v>2000</v>
+        <v>500</v>
       </c>
       <c r="G55">
-        <v>52</v>
+        <v>2</v>
       </c>
       <c r="H55" t="s">
-        <v>80</v>
+        <v>22</v>
       </c>
       <c r="I55" t="s">
         <v>13</v>
@@ -6698,28 +6861,28 @@
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>82</v>
+        <v>49</v>
       </c>
       <c r="B56" t="s">
-        <v>82</v>
+        <v>49</v>
       </c>
       <c r="C56" t="b">
         <v>1</v>
       </c>
       <c r="D56">
-        <v>104</v>
+        <v>3636</v>
       </c>
       <c r="E56">
-        <v>208</v>
+        <v>810</v>
       </c>
       <c r="F56">
-        <v>2000</v>
+        <v>500</v>
       </c>
       <c r="G56">
-        <v>52</v>
+        <v>2</v>
       </c>
       <c r="H56" t="s">
-        <v>80</v>
+        <v>22</v>
       </c>
       <c r="I56" t="s">
         <v>13</v>
@@ -6733,69 +6896,69 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="B57" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="C57" t="b">
         <v>1</v>
       </c>
       <c r="D57">
-        <v>105</v>
+        <v>180</v>
       </c>
       <c r="E57">
-        <v>105</v>
+        <v>180</v>
       </c>
       <c r="F57">
-        <v>144</v>
+        <v>45</v>
       </c>
       <c r="G57">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="H57" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="I57" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J57">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K57" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>84</v>
+        <v>14</v>
       </c>
       <c r="B58" t="s">
-        <v>84</v>
+        <v>14</v>
       </c>
       <c r="C58" t="b">
         <v>1</v>
       </c>
       <c r="D58">
-        <v>180</v>
+        <v>15</v>
       </c>
       <c r="E58">
-        <v>180</v>
+        <v>15</v>
       </c>
       <c r="F58">
-        <v>144</v>
+        <v>640</v>
       </c>
       <c r="G58">
+        <v>3</v>
+      </c>
+      <c r="H58" t="s">
+        <v>15</v>
+      </c>
+      <c r="I58" t="s">
+        <v>16</v>
+      </c>
+      <c r="J58">
         <v>2</v>
-      </c>
-      <c r="H58" t="s">
-        <v>12</v>
-      </c>
-      <c r="I58" t="s">
-        <v>13</v>
-      </c>
-      <c r="J58">
-        <v>1</v>
       </c>
       <c r="K58" t="b">
         <v>1</v>
@@ -6803,25 +6966,25 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>85</v>
+        <v>55</v>
       </c>
       <c r="B59" t="s">
-        <v>85</v>
+        <v>55</v>
       </c>
       <c r="C59" t="b">
         <v>1</v>
       </c>
       <c r="D59">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E59">
+        <v>850</v>
+      </c>
+      <c r="F59">
         <v>152</v>
       </c>
-      <c r="F59">
-        <v>30</v>
-      </c>
       <c r="G59">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="H59" t="s">
         <v>18</v>
@@ -6830,42 +6993,42 @@
         <v>16</v>
       </c>
       <c r="J59">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="K59" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="B60" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="C60" t="b">
         <v>1</v>
       </c>
       <c r="D60">
-        <v>375</v>
+        <v>2238</v>
       </c>
       <c r="E60">
-        <v>375</v>
+        <v>2241</v>
       </c>
       <c r="F60">
-        <v>720</v>
+        <v>315</v>
       </c>
       <c r="G60">
+        <v>8</v>
+      </c>
+      <c r="H60" t="s">
+        <v>18</v>
+      </c>
+      <c r="I60" t="s">
+        <v>16</v>
+      </c>
+      <c r="J60">
         <v>3</v>
-      </c>
-      <c r="H60" t="s">
-        <v>12</v>
-      </c>
-      <c r="I60" t="s">
-        <v>13</v>
-      </c>
-      <c r="J60">
-        <v>1</v>
       </c>
       <c r="K60" t="b">
         <v>1</v>
@@ -6873,34 +7036,34 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>87</v>
+        <v>39</v>
       </c>
       <c r="B61" t="s">
-        <v>87</v>
+        <v>39</v>
       </c>
       <c r="C61" t="b">
         <v>1</v>
       </c>
       <c r="D61">
-        <v>20</v>
+        <v>137</v>
       </c>
       <c r="E61">
-        <v>50</v>
+        <v>138</v>
       </c>
       <c r="F61">
-        <v>2844</v>
+        <v>207</v>
       </c>
       <c r="G61">
         <v>4</v>
       </c>
       <c r="H61" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I61" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J61">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K61" t="b">
         <v>1</v>
@@ -6908,34 +7071,34 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>88</v>
+        <v>42</v>
       </c>
       <c r="B62" t="s">
-        <v>88</v>
+        <v>42</v>
       </c>
       <c r="C62" t="b">
         <v>1</v>
       </c>
       <c r="D62">
-        <v>375</v>
+        <v>261</v>
       </c>
       <c r="E62">
-        <v>375</v>
+        <v>263</v>
       </c>
       <c r="F62">
-        <v>720</v>
+        <v>1751</v>
       </c>
       <c r="G62">
+        <v>4</v>
+      </c>
+      <c r="H62" t="s">
+        <v>43</v>
+      </c>
+      <c r="I62" t="s">
+        <v>16</v>
+      </c>
+      <c r="J62">
         <v>3</v>
-      </c>
-      <c r="H62" t="s">
-        <v>12</v>
-      </c>
-      <c r="I62" t="s">
-        <v>13</v>
-      </c>
-      <c r="J62">
-        <v>1</v>
       </c>
       <c r="K62" t="b">
         <v>1</v>
@@ -6943,34 +7106,34 @@
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>89</v>
+        <v>40</v>
       </c>
       <c r="B63" t="s">
-        <v>89</v>
+        <v>41</v>
       </c>
       <c r="C63" t="b">
         <v>1</v>
       </c>
       <c r="D63">
-        <v>268</v>
+        <v>30</v>
       </c>
       <c r="E63">
-        <v>293</v>
+        <v>270</v>
       </c>
       <c r="F63">
-        <v>896</v>
+        <v>65</v>
       </c>
       <c r="G63">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H63" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="I63" t="s">
         <v>16</v>
       </c>
       <c r="J63">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K63" t="b">
         <v>1</v>
@@ -6978,34 +7141,34 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="B64" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="C64" t="b">
         <v>1</v>
       </c>
       <c r="D64">
-        <v>200</v>
+        <v>12</v>
       </c>
       <c r="E64">
-        <v>180</v>
+        <v>15</v>
       </c>
       <c r="F64">
-        <v>1152</v>
+        <v>2500</v>
       </c>
       <c r="G64">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H64" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="I64" t="s">
         <v>16</v>
       </c>
       <c r="J64">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="K64" t="b">
         <v>1</v>
@@ -7013,69 +7176,69 @@
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="B65" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="C65" t="b">
         <v>1</v>
       </c>
       <c r="D65">
-        <v>300</v>
+        <v>2459</v>
       </c>
       <c r="E65">
-        <v>600</v>
+        <v>2466</v>
       </c>
       <c r="F65">
-        <v>1500</v>
+        <v>36</v>
       </c>
       <c r="G65">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="H65" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="I65" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J65">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="K65" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>92</v>
+        <v>28</v>
       </c>
       <c r="B66" t="s">
-        <v>92</v>
+        <v>28</v>
       </c>
       <c r="C66" t="b">
         <v>1</v>
       </c>
       <c r="D66">
-        <v>450</v>
+        <v>108</v>
       </c>
       <c r="E66">
-        <v>450</v>
+        <v>72</v>
       </c>
       <c r="F66">
-        <v>1500</v>
+        <v>1197</v>
       </c>
       <c r="G66">
+        <v>12</v>
+      </c>
+      <c r="H66" t="s">
+        <v>18</v>
+      </c>
+      <c r="I66" t="s">
+        <v>16</v>
+      </c>
+      <c r="J66">
         <v>6</v>
-      </c>
-      <c r="H66" t="s">
-        <v>20</v>
-      </c>
-      <c r="I66" t="s">
-        <v>13</v>
-      </c>
-      <c r="J66">
-        <v>1</v>
       </c>
       <c r="K66" t="b">
         <v>1</v>
@@ -7083,34 +7246,34 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>93</v>
+        <v>17</v>
       </c>
       <c r="B67" t="s">
-        <v>93</v>
+        <v>17</v>
       </c>
       <c r="C67" t="b">
         <v>1</v>
       </c>
       <c r="D67">
-        <v>450</v>
+        <v>40</v>
       </c>
       <c r="E67">
-        <v>450</v>
+        <v>40</v>
       </c>
       <c r="F67">
-        <v>1500</v>
+        <v>100</v>
       </c>
       <c r="G67">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H67" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I67" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J67">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="K67" t="b">
         <v>1</v>
@@ -7118,34 +7281,34 @@
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="B68" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C68" t="b">
         <v>1</v>
       </c>
       <c r="D68">
-        <v>375</v>
+        <v>151</v>
       </c>
       <c r="E68">
-        <v>375</v>
+        <v>152</v>
       </c>
       <c r="F68">
-        <v>720</v>
+        <v>30</v>
       </c>
       <c r="G68">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H68" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="I68" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J68">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="K68" t="b">
         <v>1</v>
@@ -7153,69 +7316,69 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B69" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C69" t="b">
         <v>1</v>
       </c>
       <c r="D69">
-        <v>20</v>
+        <v>268</v>
       </c>
       <c r="E69">
-        <v>601</v>
+        <v>293</v>
       </c>
       <c r="F69">
-        <v>70</v>
+        <v>896</v>
       </c>
       <c r="G69">
         <v>2</v>
       </c>
       <c r="H69" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="I69" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J69">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="K69" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B70" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C70" t="b">
         <v>1</v>
       </c>
       <c r="D70">
-        <v>27</v>
+        <v>200</v>
       </c>
       <c r="E70">
-        <v>953</v>
+        <v>180</v>
       </c>
       <c r="F70">
-        <v>65</v>
+        <v>1152</v>
       </c>
       <c r="G70">
         <v>2</v>
       </c>
       <c r="H70" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="I70" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J70">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="K70" t="b">
         <v>1</v>
@@ -7223,34 +7386,34 @@
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>97</v>
+        <v>54</v>
       </c>
       <c r="B71" t="s">
-        <v>97</v>
+        <v>54</v>
       </c>
       <c r="C71" t="b">
         <v>1</v>
       </c>
       <c r="D71">
-        <v>12</v>
+        <v>160</v>
       </c>
       <c r="E71">
-        <v>15</v>
+        <v>74</v>
       </c>
       <c r="F71">
-        <v>2500</v>
+        <v>400</v>
       </c>
       <c r="G71">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H71" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="I71" t="s">
         <v>16</v>
       </c>
       <c r="J71">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="K71" t="b">
         <v>1</v>
@@ -7258,69 +7421,69 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>98</v>
+        <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>98</v>
+        <v>71</v>
       </c>
       <c r="C72" t="b">
         <v>1</v>
       </c>
       <c r="D72">
-        <v>1000</v>
+        <v>180</v>
       </c>
       <c r="E72">
-        <v>8236</v>
+        <v>180</v>
       </c>
       <c r="F72">
-        <v>1024</v>
+        <v>51</v>
       </c>
       <c r="G72">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H72" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="I72" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J72">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="K72" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>99</v>
+        <v>47</v>
       </c>
       <c r="B73" t="s">
-        <v>99</v>
+        <v>47</v>
       </c>
       <c r="C73" t="b">
         <v>1</v>
       </c>
       <c r="D73">
-        <v>613</v>
+        <v>316</v>
       </c>
       <c r="E73">
-        <v>370</v>
+        <v>100</v>
       </c>
       <c r="F73">
-        <v>235</v>
+        <v>50</v>
       </c>
       <c r="G73">
         <v>2</v>
       </c>
       <c r="H73" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="I73" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J73">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="K73" t="b">
         <v>1</v>
@@ -7328,69 +7491,69 @@
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>100</v>
+        <v>56</v>
       </c>
       <c r="B74" t="s">
-        <v>100</v>
+        <v>56</v>
       </c>
       <c r="C74" t="b">
         <v>1</v>
       </c>
       <c r="D74">
-        <v>100</v>
+        <v>204</v>
       </c>
       <c r="E74">
-        <v>100</v>
+        <v>205</v>
       </c>
       <c r="F74">
-        <v>275</v>
+        <v>405</v>
       </c>
       <c r="G74">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H74" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="I74" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J74">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="K74" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>101</v>
+        <v>70</v>
       </c>
       <c r="B75" t="s">
-        <v>101</v>
+        <v>70</v>
       </c>
       <c r="C75" t="b">
         <v>1</v>
       </c>
       <c r="D75">
-        <v>23</v>
+        <v>278</v>
       </c>
       <c r="E75">
-        <v>1139</v>
+        <v>100</v>
       </c>
       <c r="F75">
-        <v>82</v>
+        <v>3000</v>
       </c>
       <c r="G75">
         <v>2</v>
       </c>
       <c r="H75" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="I75" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J75">
-        <v>1</v>
+        <v>64</v>
       </c>
       <c r="K75" t="b">
         <v>1</v>
@@ -7398,34 +7561,34 @@
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>102</v>
+        <v>45</v>
       </c>
       <c r="B76" t="s">
-        <v>102</v>
+        <v>45</v>
       </c>
       <c r="C76" t="b">
         <v>1</v>
       </c>
       <c r="D76">
-        <v>2238</v>
+        <v>5890</v>
       </c>
       <c r="E76">
-        <v>2241</v>
+        <v>3524</v>
       </c>
       <c r="F76">
-        <v>315</v>
+        <v>62</v>
       </c>
       <c r="G76">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="H76" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="I76" t="s">
         <v>16</v>
       </c>
       <c r="J76">
-        <v>3</v>
+        <v>144</v>
       </c>
       <c r="K76" t="b">
         <v>1</v>
@@ -7433,69 +7596,69 @@
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="C77" t="b">
         <v>1</v>
       </c>
       <c r="D77">
-        <v>1000</v>
+        <v>267</v>
       </c>
       <c r="E77">
-        <v>6164</v>
+        <v>173</v>
       </c>
       <c r="F77">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="G77">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H77" t="s">
-        <v>22</v>
+        <v>76</v>
       </c>
       <c r="I77" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J77">
-        <v>1</v>
+        <v>963</v>
       </c>
       <c r="K77" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>104</v>
+        <v>29</v>
       </c>
       <c r="B78" t="s">
-        <v>104</v>
+        <v>29</v>
       </c>
       <c r="C78" t="b">
         <v>1</v>
       </c>
       <c r="D78">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E78">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F78">
-        <v>234</v>
+        <v>270</v>
       </c>
       <c r="G78">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H78" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="I78" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J78">
-        <v>1</v>
+        <v>1345</v>
       </c>
       <c r="K78" t="b">
         <v>1</v>

</xml_diff>